<commit_message>
Further exploration of pre-election models. Capture and export covariance matrices and coefficient means, for use in setting post-election priors.
</commit_message>
<xml_diff>
--- a/Data/Label translations.xlsx
+++ b/Data/Label translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Apparatchiq/Desktop/Bamberg 2019/Bayes_project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5607CA7-6643-BE42-9927-1CF8C25FC056}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16E958D-F3C7-E647-BA3D-9178FDEACD56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1020" windowWidth="27640" windowHeight="13460" xr2:uid="{24EEAEA6-BE72-3E4F-B567-B654F7637CA3}"/>
+    <workbookView xWindow="2000" yWindow="460" windowWidth="27640" windowHeight="13460" xr2:uid="{24EEAEA6-BE72-3E4F-B567-B654F7637CA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>Verfügbares Einkommen der privaten Haushalte 2014 (€ je Einwohner)</t>
   </si>
   <si>
-    <t>Bruttoinlandsprodukt 2014 (€ je Einwohner)</t>
-  </si>
-  <si>
     <t>Kraftfahrzeugbestand am 01.01.2016 (je 1000 Einwohner)</t>
   </si>
   <si>
@@ -477,9 +474,6 @@
     <t>Pop_Germans_Count</t>
   </si>
   <si>
-    <t>Pop_Total_Cout</t>
-  </si>
-  <si>
     <t>EnglishTrans</t>
   </si>
   <si>
@@ -489,7 +483,13 @@
     <t>EnglishShort</t>
   </si>
   <si>
-    <t>Educ_Fachhoch_Pct</t>
+    <t>Educ_UnivQualif_Pct</t>
+  </si>
+  <si>
+    <t>§</t>
+  </si>
+  <si>
+    <t>Pop_Total_Count</t>
   </si>
 </sst>
 </file>
@@ -850,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D23CFD-82C6-5249-A9FC-84BBDF62E210}">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -863,29 +863,29 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
         <v>151</v>
-      </c>
-      <c r="B1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -896,541 +896,541 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>153</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C51" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C52" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>